<commit_message>
Added scrum master task to in process
</commit_message>
<xml_diff>
--- a/burndown/Team Blue Burndown Chart.xlsx
+++ b/burndown/Team Blue Burndown Chart.xlsx
@@ -1219,6 +1219,18 @@
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1257,18 +1269,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1279,54 +1279,7 @@
     <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color theme="1"/>
@@ -1492,16 +1445,16 @@
                   <c:v>29.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.75</c:v>
+                  <c:v>20.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.75</c:v>
+                  <c:v>20.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.75</c:v>
+                  <c:v>20.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21.75</c:v>
+                  <c:v>20.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2060,8 +2013,8 @@
   </sheetPr>
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2077,57 +2030,57 @@
   <sheetData>
     <row r="1" spans="1:23" ht="49.8" x14ac:dyDescent="0.8">
       <c r="A1" s="24"/>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="79"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="83"/>
     </row>
     <row r="2" spans="1:23" ht="33" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="24"/>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="80"/>
-      <c r="U2" s="80"/>
-      <c r="V2" s="80"/>
-      <c r="W2" s="80"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="84"/>
+      <c r="T2" s="84"/>
+      <c r="U2" s="84"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="84"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="22"/>
@@ -2135,20 +2088,20 @@
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
-      <c r="F3" s="81" t="s">
+      <c r="F3" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="84" t="s">
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="86"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="90"/>
       <c r="P3" s="62"/>
       <c r="Q3" s="31"/>
       <c r="R3" s="31"/>
@@ -2282,13 +2235,13 @@
         <f t="shared" ref="P6:P25" si="0">IF(D6="","-",(IF(COUNT(E6:O6) = 0,"To Do",IF(E6&gt;SUM(F6:O6),"Incomplete","Done"))))</f>
         <v>Done</v>
       </c>
-      <c r="R6" s="87" t="s">
+      <c r="R6" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="90"/>
-      <c r="T6" s="90"/>
-      <c r="U6" s="90"/>
-      <c r="V6" s="91"/>
+      <c r="S6" s="94"/>
+      <c r="T6" s="94"/>
+      <c r="U6" s="94"/>
+      <c r="V6" s="95"/>
       <c r="W6" s="10"/>
     </row>
     <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.35">
@@ -2584,13 +2537,13 @@
         <v>Done</v>
       </c>
       <c r="Q14" s="8"/>
-      <c r="R14" s="87" t="s">
+      <c r="R14" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="S14" s="90"/>
-      <c r="T14" s="90"/>
-      <c r="U14" s="90"/>
-      <c r="V14" s="91"/>
+      <c r="S14" s="94"/>
+      <c r="T14" s="94"/>
+      <c r="U14" s="94"/>
+      <c r="V14" s="95"/>
       <c r="W14" s="10"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
@@ -2627,10 +2580,10 @@
       </c>
       <c r="Q15" s="44"/>
       <c r="R15" s="70"/>
-      <c r="S15" s="92" t="s">
+      <c r="S15" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="T15" s="92"/>
+      <c r="T15" s="79"/>
       <c r="U15" s="44">
         <f>SUM(E6:E25)</f>
         <v>45.5</v>
@@ -2674,10 +2627,10 @@
       </c>
       <c r="Q16" s="44"/>
       <c r="R16" s="70"/>
-      <c r="S16" s="93" t="s">
+      <c r="S16" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="T16" s="93"/>
+      <c r="T16" s="80"/>
       <c r="U16" s="44">
         <f>SUMIF(F6:O25,"&lt;0")*-1</f>
         <v>34.5</v>
@@ -2714,11 +2667,11 @@
         <v>Done</v>
       </c>
       <c r="Q17" s="44"/>
-      <c r="R17" s="94" t="s">
+      <c r="R17" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="S17" s="95"/>
-      <c r="T17" s="95"/>
+      <c r="S17" s="82"/>
+      <c r="T17" s="82"/>
       <c r="U17" s="75">
         <f>SUM(U15,U16)</f>
         <v>80</v>
@@ -2855,13 +2808,13 @@
         <v>Incomplete</v>
       </c>
       <c r="Q21" s="44"/>
-      <c r="R21" s="87" t="s">
+      <c r="R21" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="S21" s="88"/>
-      <c r="T21" s="88"/>
-      <c r="U21" s="88"/>
-      <c r="V21" s="89"/>
+      <c r="S21" s="92"/>
+      <c r="T21" s="92"/>
+      <c r="U21" s="92"/>
+      <c r="V21" s="93"/>
       <c r="W21" s="10"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
@@ -2892,10 +2845,10 @@
       </c>
       <c r="Q22" s="44"/>
       <c r="R22" s="70"/>
-      <c r="S22" s="92" t="s">
+      <c r="S22" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="T22" s="92"/>
+      <c r="T22" s="79"/>
       <c r="U22" s="44">
         <f>SUMIF(F6:J25,"&gt;0")</f>
         <v>35.5</v>
@@ -2927,13 +2880,13 @@
       </c>
       <c r="Q23" s="44"/>
       <c r="R23" s="70"/>
-      <c r="S23" s="93" t="s">
+      <c r="S23" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="T23" s="93"/>
+      <c r="T23" s="80"/>
       <c r="U23" s="78">
         <f>SUMIF(K6:O25,"&gt;0")</f>
-        <v>22.75</v>
+        <v>23.75</v>
       </c>
       <c r="V23" s="71"/>
       <c r="W23" s="10"/>
@@ -2957,7 +2910,7 @@
         <v>-8</v>
       </c>
       <c r="L24">
-        <v>0.75</v>
+        <v>1.75</v>
       </c>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
@@ -2967,14 +2920,14 @@
         <v>Incomplete</v>
       </c>
       <c r="Q24" s="44"/>
-      <c r="R24" s="94" t="s">
+      <c r="R24" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="S24" s="95"/>
-      <c r="T24" s="95"/>
+      <c r="S24" s="82"/>
+      <c r="T24" s="82"/>
       <c r="U24" s="77">
         <f>SUM(U22,U23)</f>
-        <v>58.25</v>
+        <v>59.25</v>
       </c>
       <c r="V24" s="71"/>
       <c r="W24" s="10"/>
@@ -3066,19 +3019,19 @@
       </c>
       <c r="L26" s="50">
         <f t="shared" si="1"/>
-        <v>21.75</v>
+        <v>20.75</v>
       </c>
       <c r="M26" s="50">
         <f t="shared" si="1"/>
-        <v>21.75</v>
+        <v>20.75</v>
       </c>
       <c r="N26" s="50">
         <f t="shared" si="1"/>
-        <v>21.75</v>
+        <v>20.75</v>
       </c>
       <c r="O26" s="50">
         <f t="shared" si="1"/>
-        <v>21.75</v>
+        <v>20.75</v>
       </c>
       <c r="P26" s="53"/>
       <c r="Q26" s="44"/>
@@ -3439,12 +3392,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="13">
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S16:T16"/>
     <mergeCell ref="B1:W1"/>
     <mergeCell ref="B2:W2"/>
     <mergeCell ref="F3:J3"/>
@@ -3452,17 +3399,23 @@
     <mergeCell ref="R21:V21"/>
     <mergeCell ref="R6:V6"/>
     <mergeCell ref="R14:V14"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
   </mergeCells>
   <conditionalFormatting sqref="P6:P25">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="Incomplete">
+    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="Incomplete">
       <formula>NOT(ISERROR(SEARCH("Incomplete",P6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="2" priority="9" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",P6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6:P25">
-    <cfRule type="cellIs" dxfId="6" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Reverted ashmita's commit, fixed a typo in Model that caused the issue
</commit_message>
<xml_diff>
--- a/burndown/Team Blue Burndown Chart.xlsx
+++ b/burndown/Team Blue Burndown Chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbui1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbui1\Documents\GitHub\swe443\SWE443BankSystemBlue\burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1219,6 +1219,45 @@
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1230,45 +1269,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1445,16 +1445,16 @@
                   <c:v>29.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.75</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.75</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.75</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.75</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2013,8 +2013,8 @@
   </sheetPr>
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2030,57 +2030,57 @@
   <sheetData>
     <row r="1" spans="1:23" ht="49.8" x14ac:dyDescent="0.8">
       <c r="A1" s="24"/>
-      <c r="B1" s="83" t="s">
+      <c r="B1" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="83"/>
-      <c r="W1" s="83"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="79"/>
     </row>
     <row r="2" spans="1:23" ht="33" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="24"/>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="84"/>
-      <c r="R2" s="84"/>
-      <c r="S2" s="84"/>
-      <c r="T2" s="84"/>
-      <c r="U2" s="84"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="84"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="80"/>
+      <c r="U2" s="80"/>
+      <c r="V2" s="80"/>
+      <c r="W2" s="80"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="22"/>
@@ -2088,20 +2088,20 @@
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
-      <c r="F3" s="85" t="s">
+      <c r="F3" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="88" t="s">
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="90"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="86"/>
       <c r="P3" s="62"/>
       <c r="Q3" s="31"/>
       <c r="R3" s="31"/>
@@ -2235,13 +2235,13 @@
         <f t="shared" ref="P6:P25" si="0">IF(D6="","-",(IF(COUNT(E6:O6) = 0,"To Do",IF(E6&gt;SUM(F6:O6),"Incomplete","Done"))))</f>
         <v>Done</v>
       </c>
-      <c r="R6" s="91" t="s">
+      <c r="R6" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="94"/>
-      <c r="T6" s="94"/>
-      <c r="U6" s="94"/>
-      <c r="V6" s="95"/>
+      <c r="S6" s="90"/>
+      <c r="T6" s="90"/>
+      <c r="U6" s="90"/>
+      <c r="V6" s="91"/>
       <c r="W6" s="10"/>
     </row>
     <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.35">
@@ -2537,13 +2537,13 @@
         <v>Done</v>
       </c>
       <c r="Q14" s="8"/>
-      <c r="R14" s="91" t="s">
+      <c r="R14" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="S14" s="94"/>
-      <c r="T14" s="94"/>
-      <c r="U14" s="94"/>
-      <c r="V14" s="95"/>
+      <c r="S14" s="90"/>
+      <c r="T14" s="90"/>
+      <c r="U14" s="90"/>
+      <c r="V14" s="91"/>
       <c r="W14" s="10"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
@@ -2580,10 +2580,10 @@
       </c>
       <c r="Q15" s="44"/>
       <c r="R15" s="70"/>
-      <c r="S15" s="79" t="s">
+      <c r="S15" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="T15" s="79"/>
+      <c r="T15" s="92"/>
       <c r="U15" s="44">
         <f>SUM(E6:E25)</f>
         <v>45.5</v>
@@ -2627,10 +2627,10 @@
       </c>
       <c r="Q16" s="44"/>
       <c r="R16" s="70"/>
-      <c r="S16" s="80" t="s">
+      <c r="S16" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="T16" s="80"/>
+      <c r="T16" s="93"/>
       <c r="U16" s="44">
         <f>SUMIF(F6:O25,"&lt;0")*-1</f>
         <v>34.5</v>
@@ -2667,11 +2667,11 @@
         <v>Done</v>
       </c>
       <c r="Q17" s="44"/>
-      <c r="R17" s="81" t="s">
+      <c r="R17" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="S17" s="82"/>
-      <c r="T17" s="82"/>
+      <c r="S17" s="95"/>
+      <c r="T17" s="95"/>
       <c r="U17" s="75">
         <f>SUM(U15,U16)</f>
         <v>80</v>
@@ -2771,7 +2771,9 @@
         <v>-6</v>
       </c>
       <c r="L20" s="63"/>
-      <c r="M20" s="3"/>
+      <c r="M20" s="3">
+        <v>2</v>
+      </c>
       <c r="N20" s="3"/>
       <c r="O20" s="18"/>
       <c r="P20" s="76" t="str">
@@ -2808,13 +2810,13 @@
         <v>Incomplete</v>
       </c>
       <c r="Q21" s="44"/>
-      <c r="R21" s="91" t="s">
+      <c r="R21" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="S21" s="92"/>
-      <c r="T21" s="92"/>
-      <c r="U21" s="92"/>
-      <c r="V21" s="93"/>
+      <c r="S21" s="88"/>
+      <c r="T21" s="88"/>
+      <c r="U21" s="88"/>
+      <c r="V21" s="89"/>
       <c r="W21" s="10"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
@@ -2845,10 +2847,10 @@
       </c>
       <c r="Q22" s="44"/>
       <c r="R22" s="70"/>
-      <c r="S22" s="79" t="s">
+      <c r="S22" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="T22" s="79"/>
+      <c r="T22" s="92"/>
       <c r="U22" s="44">
         <f>SUMIF(F6:J25,"&gt;0")</f>
         <v>35.5</v>
@@ -2880,13 +2882,13 @@
       </c>
       <c r="Q23" s="44"/>
       <c r="R23" s="70"/>
-      <c r="S23" s="80" t="s">
+      <c r="S23" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="T23" s="80"/>
+      <c r="T23" s="93"/>
       <c r="U23" s="78">
         <f>SUMIF(K6:O25,"&gt;0")</f>
-        <v>23.75</v>
+        <v>27.5</v>
       </c>
       <c r="V23" s="71"/>
       <c r="W23" s="10"/>
@@ -2910,9 +2912,11 @@
         <v>-8</v>
       </c>
       <c r="L24">
-        <v>1.75</v>
-      </c>
-      <c r="M24" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="M24" s="3">
+        <v>1</v>
+      </c>
       <c r="N24" s="3"/>
       <c r="O24" s="18"/>
       <c r="P24" s="76" t="str">
@@ -2920,14 +2924,14 @@
         <v>Incomplete</v>
       </c>
       <c r="Q24" s="44"/>
-      <c r="R24" s="81" t="s">
+      <c r="R24" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="S24" s="82"/>
-      <c r="T24" s="82"/>
+      <c r="S24" s="95"/>
+      <c r="T24" s="95"/>
       <c r="U24" s="77">
         <f>SUM(U22,U23)</f>
-        <v>59.25</v>
+        <v>63</v>
       </c>
       <c r="V24" s="71"/>
       <c r="W24" s="10"/>
@@ -2965,7 +2969,9 @@
       <c r="L25" s="19">
         <v>0.5</v>
       </c>
-      <c r="M25" s="19"/>
+      <c r="M25" s="19">
+        <v>0.5</v>
+      </c>
       <c r="N25" s="19"/>
       <c r="O25" s="21"/>
       <c r="P25" s="76" t="str">
@@ -3019,19 +3025,19 @@
       </c>
       <c r="L26" s="50">
         <f t="shared" si="1"/>
-        <v>20.75</v>
+        <v>20.5</v>
       </c>
       <c r="M26" s="50">
         <f t="shared" si="1"/>
-        <v>20.75</v>
+        <v>17</v>
       </c>
       <c r="N26" s="50">
         <f t="shared" si="1"/>
-        <v>20.75</v>
+        <v>17</v>
       </c>
       <c r="O26" s="50">
         <f t="shared" si="1"/>
-        <v>20.75</v>
+        <v>17</v>
       </c>
       <c r="P26" s="53"/>
       <c r="Q26" s="44"/>
@@ -3392,6 +3398,12 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="13">
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
     <mergeCell ref="B1:W1"/>
     <mergeCell ref="B2:W2"/>
     <mergeCell ref="F3:J3"/>
@@ -3399,12 +3411,6 @@
     <mergeCell ref="R21:V21"/>
     <mergeCell ref="R6:V6"/>
     <mergeCell ref="R14:V14"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S16:T16"/>
   </mergeCells>
   <conditionalFormatting sqref="P6:P25">
     <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="Incomplete">

</xml_diff>

<commit_message>
Updated burndown chart, moved some things from kanban folders
</commit_message>
<xml_diff>
--- a/burndown/Team Blue Burndown Chart.xlsx
+++ b/burndown/Team Blue Burndown Chart.xlsx
@@ -5,23 +5,39 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbui1\Documents\GitHub\swe443\SWE443BankSystemBlue\burndown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbui1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 1.5" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sprint 1'!$C$4:$O$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sprint 1.5'!$C$4:$O$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint 2'!$C$4:$O$5</definedName>
+    <definedName name="Header" localSheetId="1">'Sprint 1.5'!$C$3:$O$5</definedName>
+    <definedName name="Header" localSheetId="2">'Sprint 2'!$C$3:$O$5</definedName>
     <definedName name="Header">'Sprint 1'!$C$3:$O$5</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Sprint 1'!$B$31:$V$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Sprint 1.5'!$B$31:$V$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Sprint 2'!$B$31:$V$40</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Sprint 1'!$3:$5</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Sprint 1.5'!$3:$5</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Sprint 2'!$3:$5</definedName>
     <definedName name="Z_FAE5DA31_FC3C_4EAB_85AB_90EFD3CA9745_.wvu.FilterData" localSheetId="0" hidden="1">'Sprint 1'!$C$4:$O$5</definedName>
+    <definedName name="Z_FAE5DA31_FC3C_4EAB_85AB_90EFD3CA9745_.wvu.FilterData" localSheetId="1" hidden="1">'Sprint 1.5'!$C$4:$O$5</definedName>
+    <definedName name="Z_FAE5DA31_FC3C_4EAB_85AB_90EFD3CA9745_.wvu.FilterData" localSheetId="2" hidden="1">'Sprint 2'!$C$4:$O$5</definedName>
     <definedName name="Z_FAE5DA31_FC3C_4EAB_85AB_90EFD3CA9745_.wvu.PrintArea" localSheetId="0" hidden="1">'Sprint 1'!$B$31:$V$40</definedName>
+    <definedName name="Z_FAE5DA31_FC3C_4EAB_85AB_90EFD3CA9745_.wvu.PrintArea" localSheetId="1" hidden="1">'Sprint 1.5'!$B$31:$V$40</definedName>
+    <definedName name="Z_FAE5DA31_FC3C_4EAB_85AB_90EFD3CA9745_.wvu.PrintArea" localSheetId="2" hidden="1">'Sprint 2'!$B$31:$V$40</definedName>
     <definedName name="Z_FAE5DA31_FC3C_4EAB_85AB_90EFD3CA9745_.wvu.PrintTitles" localSheetId="0" hidden="1">'Sprint 1'!$3:$5</definedName>
+    <definedName name="Z_FAE5DA31_FC3C_4EAB_85AB_90EFD3CA9745_.wvu.PrintTitles" localSheetId="1" hidden="1">'Sprint 1.5'!$3:$5</definedName>
+    <definedName name="Z_FAE5DA31_FC3C_4EAB_85AB_90EFD3CA9745_.wvu.PrintTitles" localSheetId="2" hidden="1">'Sprint 2'!$3:$5</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
@@ -228,6 +244,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="E23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If something is missing at the start of Sprint Planning, place this color box in column E to indicate it was added after the start of the Sprint.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Format the cell of the day that a missing item was added to the Sprint with this color and add in an estimate of story points for the item.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E24" authorId="0" shapeId="0">
       <text>
         <r>
@@ -260,8 +304,132 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Anne</author>
+  </authors>
+  <commentList>
+    <comment ref="E5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Note:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Effort calculated using Story Points assigned at Sprint Planning - Enter as a positive Integer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If something is missing at the start of Sprint Planning, place this color box in column E to indicate it was added after the start of the Sprint.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Format the cell of the day that a missing item was added to the Sprint with this color and add in an estimate of story points for the item.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Anne</author>
+  </authors>
+  <commentList>
+    <comment ref="E5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Note:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Effort calculated using Story Points assigned at Sprint Planning - Enter as a positive Integer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If something is missing at the start of Sprint Planning, place this color box in column E to indicate it was added after the start of the Sprint.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Format the cell of the day that a missing item was added to the Sprint with this color and add in an estimate of story points for the item.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="67">
   <si>
     <t>Initial 
 Estimate</t>
@@ -393,9 +561,6 @@
     <t>Class Diagram</t>
   </si>
   <si>
-    <t>Transaction Class Stub</t>
-  </si>
-  <si>
     <t>Progress</t>
   </si>
   <si>
@@ -403,6 +568,69 @@
   </si>
   <si>
     <t>Persistence Layer (includes create account, deposit, withdraw, transfer)</t>
+  </si>
+  <si>
+    <t>Transaction Log</t>
+  </si>
+  <si>
+    <t>31-2</t>
+  </si>
+  <si>
+    <t>Transaction Fee</t>
+  </si>
+  <si>
+    <t>Transaction Sequence Diagram</t>
+  </si>
+  <si>
+    <t>Research Networking/Concurrency</t>
+  </si>
+  <si>
+    <t>Sales Pitch/Presentation Planning and Completion</t>
+  </si>
+  <si>
+    <t>14-16 Apr</t>
+  </si>
+  <si>
+    <t>7-9 Apr</t>
+  </si>
+  <si>
+    <t>Scenario Writing (Transaction Log)</t>
+  </si>
+  <si>
+    <t>General Refactoring (Classes, Tests)</t>
+  </si>
+  <si>
+    <t>Modify Transaction (Undo)</t>
+  </si>
+  <si>
+    <t>Android Integration + Start Android GUI</t>
+  </si>
+  <si>
+    <t>21-23 Apr</t>
+  </si>
+  <si>
+    <t>28-30 Apr</t>
+  </si>
+  <si>
+    <t>Transaction Log + Transaction Class</t>
+  </si>
+  <si>
+    <t>Finalizing Presentation Plans (Scripts/Scenarios/Bug Fixing)</t>
+  </si>
+  <si>
+    <t>Spend time configuring git with our Android project</t>
+  </si>
+  <si>
+    <t>Continue Integrating Completed Code to Android GUI</t>
+  </si>
+  <si>
+    <t>Security (still needs estimate)</t>
+  </si>
+  <si>
+    <t>Concurrency (still needs estimate)</t>
+  </si>
+  <si>
+    <t>Networking (still needs estimate)</t>
   </si>
 </sst>
 </file>
@@ -586,7 +814,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -1060,6 +1288,34 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1073,7 +1329,7 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1219,6 +1475,34 @@
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="29" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="40" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1258,18 +1542,6 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent2" xfId="1" builtinId="35"/>
@@ -1279,7 +1551,87 @@
     <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -1442,19 +1794,19 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.25</c:v>
+                  <c:v>35.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>20.5</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>17</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>17</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1643,6 +1995,626 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SWE</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 443 Blue Bank Sprint 1.5</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 1.5'!$D$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Hours</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1.5'!$E$26:$O$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-23BE-4F66-89FA-BC1FEEDA9BFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 1.5'!$D$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1.5'!$E$27:$O$27</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-23BE-4F66-89FA-BC1FEEDA9BFB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="414553768"/>
+        <c:axId val="414555728"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="414553768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="414555728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="414555728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="414553768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SWE</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 443 Blue Bank Sprint 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$D$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Hours</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$E$26:$O$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3862-4FE9-8CFC-9671FFF711EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$D$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal Trend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$E$27:$O$27</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.6000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4000000000000021</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000018</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.8000000000000016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.6000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.4000000000000012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2000000000000013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3862-4FE9-8CFC-9671FFF711EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="414553768"/>
+        <c:axId val="414555728"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="414553768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="414555728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="414555728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="414553768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1664,6 +2636,92 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E240000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2108587</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>108189</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>145877</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>136318</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8751BCD-74AC-4D64-82F6-D9A7BE97F6F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2108587</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>108189</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>145877</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>136318</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8CAC424-AA93-4898-A2A3-B1465C129943}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2013,8 +3071,8 @@
   </sheetPr>
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2030,57 +3088,57 @@
   <sheetData>
     <row r="1" spans="1:23" ht="49.8" x14ac:dyDescent="0.8">
       <c r="A1" s="24"/>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="79"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="89"/>
+      <c r="T1" s="89"/>
+      <c r="U1" s="89"/>
+      <c r="V1" s="89"/>
+      <c r="W1" s="89"/>
     </row>
     <row r="2" spans="1:23" ht="33" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="24"/>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="80"/>
-      <c r="U2" s="80"/>
-      <c r="V2" s="80"/>
-      <c r="W2" s="80"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="90"/>
+      <c r="W2" s="90"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="22"/>
@@ -2088,20 +3146,20 @@
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
-      <c r="F3" s="81" t="s">
+      <c r="F3" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="84" t="s">
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="86"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="96"/>
       <c r="P3" s="62"/>
       <c r="Q3" s="31"/>
       <c r="R3" s="31"/>
@@ -2136,8 +3194,8 @@
       <c r="J4" s="55">
         <v>42824</v>
       </c>
-      <c r="K4" s="42">
-        <v>42825</v>
+      <c r="K4" s="42" t="s">
+        <v>47</v>
       </c>
       <c r="L4" s="43">
         <v>42828</v>
@@ -2235,13 +3293,13 @@
         <f t="shared" ref="P6:P25" si="0">IF(D6="","-",(IF(COUNT(E6:O6) = 0,"To Do",IF(E6&gt;SUM(F6:O6),"Incomplete","Done"))))</f>
         <v>Done</v>
       </c>
-      <c r="R6" s="87" t="s">
+      <c r="R6" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="90"/>
-      <c r="T6" s="90"/>
-      <c r="U6" s="90"/>
-      <c r="V6" s="91"/>
+      <c r="S6" s="100"/>
+      <c r="T6" s="100"/>
+      <c r="U6" s="100"/>
+      <c r="V6" s="101"/>
       <c r="W6" s="10"/>
     </row>
     <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.35">
@@ -2537,13 +3595,13 @@
         <v>Done</v>
       </c>
       <c r="Q14" s="8"/>
-      <c r="R14" s="87" t="s">
-        <v>45</v>
-      </c>
-      <c r="S14" s="90"/>
-      <c r="T14" s="90"/>
-      <c r="U14" s="90"/>
-      <c r="V14" s="91"/>
+      <c r="R14" s="97" t="s">
+        <v>44</v>
+      </c>
+      <c r="S14" s="100"/>
+      <c r="T14" s="100"/>
+      <c r="U14" s="100"/>
+      <c r="V14" s="101"/>
       <c r="W14" s="10"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
@@ -2553,7 +3611,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="3"/>
@@ -2580,10 +3638,10 @@
       </c>
       <c r="Q15" s="44"/>
       <c r="R15" s="70"/>
-      <c r="S15" s="92" t="s">
+      <c r="S15" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="T15" s="92"/>
+      <c r="T15" s="85"/>
       <c r="U15" s="44">
         <f>SUM(E6:E25)</f>
         <v>45.5</v>
@@ -2627,13 +3685,13 @@
       </c>
       <c r="Q16" s="44"/>
       <c r="R16" s="70"/>
-      <c r="S16" s="93" t="s">
+      <c r="S16" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="T16" s="93"/>
+      <c r="T16" s="86"/>
       <c r="U16" s="44">
         <f>SUMIF(F6:O25,"&lt;0")*-1</f>
-        <v>34.5</v>
+        <v>42.5</v>
       </c>
       <c r="V16" s="71"/>
       <c r="W16" s="10"/>
@@ -2667,14 +3725,14 @@
         <v>Done</v>
       </c>
       <c r="Q17" s="44"/>
-      <c r="R17" s="94" t="s">
+      <c r="R17" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="S17" s="95"/>
-      <c r="T17" s="95"/>
+      <c r="S17" s="88"/>
+      <c r="T17" s="88"/>
       <c r="U17" s="75">
         <f>SUM(U15,U16)</f>
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="V17" s="71"/>
       <c r="W17" s="10"/>
@@ -2698,14 +3756,16 @@
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
+      <c r="K18" s="3">
+        <v>1</v>
+      </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="18"/>
       <c r="P18" s="76" t="str">
         <f t="shared" si="0"/>
-        <v>Incomplete</v>
+        <v>Done</v>
       </c>
       <c r="Q18" s="44"/>
       <c r="R18" s="72"/>
@@ -2774,11 +3834,15 @@
       <c r="M20" s="3">
         <v>2</v>
       </c>
-      <c r="N20" s="3"/>
-      <c r="O20" s="18"/>
+      <c r="N20" s="3">
+        <v>2</v>
+      </c>
+      <c r="O20" s="18">
+        <v>2</v>
+      </c>
       <c r="P20" s="76" t="str">
         <f t="shared" si="0"/>
-        <v>Incomplete</v>
+        <v>Done</v>
       </c>
       <c r="Q20" s="44"/>
       <c r="W20" s="10"/>
@@ -2810,13 +3874,13 @@
         <v>Incomplete</v>
       </c>
       <c r="Q21" s="44"/>
-      <c r="R21" s="87" t="s">
-        <v>44</v>
-      </c>
-      <c r="S21" s="88"/>
-      <c r="T21" s="88"/>
-      <c r="U21" s="88"/>
-      <c r="V21" s="89"/>
+      <c r="R21" s="97" t="s">
+        <v>43</v>
+      </c>
+      <c r="S21" s="98"/>
+      <c r="T21" s="98"/>
+      <c r="U21" s="98"/>
+      <c r="V21" s="99"/>
       <c r="W21" s="10"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
@@ -2826,7 +3890,7 @@
         <v>17</v>
       </c>
       <c r="D22" s="65" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="3"/>
@@ -2835,22 +3899,24 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="45">
-        <v>-1</v>
+        <v>-8</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
-      <c r="O22" s="18"/>
+      <c r="O22" s="18">
+        <v>0.5</v>
+      </c>
       <c r="P22" s="76" t="str">
         <f t="shared" si="0"/>
         <v>Incomplete</v>
       </c>
       <c r="Q22" s="44"/>
       <c r="R22" s="70"/>
-      <c r="S22" s="92" t="s">
+      <c r="S22" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="T22" s="92"/>
+      <c r="T22" s="85"/>
       <c r="U22" s="44">
         <f>SUMIF(F6:J25,"&gt;0")</f>
         <v>35.5</v>
@@ -2864,8 +3930,10 @@
       <c r="C23" s="51">
         <v>18</v>
       </c>
-      <c r="D23" s="65"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="4"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -2873,22 +3941,26 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
+      <c r="M23" s="45">
+        <v>-1</v>
+      </c>
+      <c r="N23" s="3">
+        <v>1</v>
+      </c>
       <c r="O23" s="18"/>
       <c r="P23" s="76" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>Done</v>
       </c>
       <c r="Q23" s="44"/>
       <c r="R23" s="70"/>
-      <c r="S23" s="93" t="s">
+      <c r="S23" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="T23" s="93"/>
+      <c r="T23" s="86"/>
       <c r="U23" s="78">
         <f>SUMIF(K6:O25,"&gt;0")</f>
-        <v>27.5</v>
+        <v>36</v>
       </c>
       <c r="V23" s="71"/>
       <c r="W23" s="10"/>
@@ -2918,20 +3990,22 @@
         <v>1</v>
       </c>
       <c r="N24" s="3"/>
-      <c r="O24" s="18"/>
+      <c r="O24" s="18">
+        <v>1</v>
+      </c>
       <c r="P24" s="76" t="str">
         <f t="shared" si="0"/>
         <v>Incomplete</v>
       </c>
       <c r="Q24" s="44"/>
-      <c r="R24" s="94" t="s">
+      <c r="R24" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="S24" s="95"/>
-      <c r="T24" s="95"/>
+      <c r="S24" s="88"/>
+      <c r="T24" s="88"/>
       <c r="U24" s="77">
         <f>SUM(U22,U23)</f>
-        <v>63</v>
+        <v>71.5</v>
       </c>
       <c r="V24" s="71"/>
       <c r="W24" s="10"/>
@@ -2972,11 +4046,15 @@
       <c r="M25" s="19">
         <v>0.5</v>
       </c>
-      <c r="N25" s="19"/>
-      <c r="O25" s="21"/>
+      <c r="N25" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="O25" s="21">
+        <v>0.5</v>
+      </c>
       <c r="P25" s="76" t="str">
         <f t="shared" si="0"/>
-        <v>Incomplete</v>
+        <v>Done</v>
       </c>
       <c r="Q25" s="44"/>
       <c r="R25" s="72"/>
@@ -3021,23 +4099,23 @@
       </c>
       <c r="K26" s="50">
         <f t="shared" si="1"/>
-        <v>29.25</v>
+        <v>35.25</v>
       </c>
       <c r="L26" s="50">
         <f t="shared" si="1"/>
-        <v>20.5</v>
+        <v>26.5</v>
       </c>
       <c r="M26" s="50">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="N26" s="50">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>20.5</v>
       </c>
       <c r="O26" s="50">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>16.5</v>
       </c>
       <c r="P26" s="53"/>
       <c r="Q26" s="44"/>
@@ -3398,12 +4476,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="13">
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="R24:T24"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S16:T16"/>
     <mergeCell ref="B1:W1"/>
     <mergeCell ref="B2:W2"/>
     <mergeCell ref="F3:J3"/>
@@ -3411,34 +4483,40 @@
     <mergeCell ref="R21:V21"/>
     <mergeCell ref="R6:V6"/>
     <mergeCell ref="R14:V14"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
   </mergeCells>
   <conditionalFormatting sqref="P6:P25">
-    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="Incomplete">
+    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="Incomplete">
       <formula>NOT(ISERROR(SEARCH("Incomplete",P6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="9" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",P6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6:P25">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" stopIfTrue="1" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S8 E14:E16 E24 E20:E22">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S8 E14:E16 E20:E24">
       <formula1>0</formula1>
       <formula2>1000000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S9:S10 I14:I15 K24 K20:K22">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S9:S10 I14:I15 K24 K20:K22 M23">
       <formula1>-100</formula1>
       <formula2>1000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H26:O27 E27 M6:O25 I8:J12 K6:L19 F8:H19 J14:J19 I16:I19 F22:G27 H22:J25 K25:L25 L22:L23 K23">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H26:O27 E27 K23 I8:J12 K6:L19 F8:H19 J14:J19 I16:I19 F22:G27 H22:J25 K25:L25 L22:L23 N6:O25 M6:M22 M24:M25">
       <formula1>-24</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E13 E17:E19 E23">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E13 E17:E19">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>
@@ -3483,4 +4561,2750 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:X42"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="66.5546875" customWidth="1"/>
+    <col min="5" max="15" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" customWidth="1"/>
+    <col min="21" max="21" width="6" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" customWidth="1"/>
+    <col min="24" max="24" width="25.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="49.8" x14ac:dyDescent="0.8">
+      <c r="A1" s="24"/>
+      <c r="B1" s="89" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="89"/>
+      <c r="T1" s="89"/>
+      <c r="U1" s="89"/>
+      <c r="V1" s="89"/>
+      <c r="W1" s="89"/>
+    </row>
+    <row r="2" spans="1:23" ht="33" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="24"/>
+      <c r="B2" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="90"/>
+      <c r="W2" s="90"/>
+    </row>
+    <row r="3" spans="1:23" s="1" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="22"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="91" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="32"/>
+    </row>
+    <row r="4" spans="1:23" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="34"/>
+      <c r="F4" s="43">
+        <v>42830</v>
+      </c>
+      <c r="G4" s="43">
+        <v>42831</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="42">
+        <v>42835</v>
+      </c>
+      <c r="J4" s="42">
+        <v>42836</v>
+      </c>
+      <c r="K4" s="42">
+        <v>42837</v>
+      </c>
+      <c r="L4" s="42">
+        <v>42838</v>
+      </c>
+      <c r="M4" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" s="43">
+        <v>42842</v>
+      </c>
+      <c r="O4" s="58">
+        <v>42843</v>
+      </c>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="W4" s="27"/>
+    </row>
+    <row r="5" spans="1:23" s="2" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="23"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="W5" s="27"/>
+    </row>
+    <row r="6" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="24"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="17">
+        <v>1</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="63">
+        <v>1</v>
+      </c>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63">
+        <v>-3</v>
+      </c>
+      <c r="H6" s="63">
+        <v>3</v>
+      </c>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="5">
+        <v>1</v>
+      </c>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="76" t="str">
+        <f t="shared" ref="P6:P25" si="0">IF(D6="","-",(IF(COUNT(E6:O6) = 0,"To Do",IF(E6&gt;SUM(F6:O6),"Incomplete","Done"))))</f>
+        <v>Done</v>
+      </c>
+      <c r="R6" s="97" t="s">
+        <v>4</v>
+      </c>
+      <c r="S6" s="100"/>
+      <c r="T6" s="100"/>
+      <c r="U6" s="100"/>
+      <c r="V6" s="101"/>
+      <c r="W6" s="10"/>
+    </row>
+    <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="24"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="17">
+        <v>2</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="63">
+        <v>2</v>
+      </c>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="3">
+        <v>2</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="R7" s="9"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+    </row>
+    <row r="8" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="17">
+        <v>3</v>
+      </c>
+      <c r="D8" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3">
+        <v>2</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="R8" s="9"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A9" s="24"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="17">
+        <v>4</v>
+      </c>
+      <c r="D9" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="3">
+        <v>8</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="K9" s="48">
+        <v>1</v>
+      </c>
+      <c r="L9" s="48"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3">
+        <v>7</v>
+      </c>
+      <c r="O9" s="18">
+        <v>1</v>
+      </c>
+      <c r="P9" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="R9" s="9"/>
+      <c r="S9" s="45"/>
+      <c r="T9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A10" s="24"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="17">
+        <v>5</v>
+      </c>
+      <c r="D10" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="R10" s="9"/>
+      <c r="S10" s="46"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+    </row>
+    <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="24"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="47">
+        <v>6</v>
+      </c>
+      <c r="D11" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="3">
+        <v>3</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3">
+        <v>2</v>
+      </c>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="18">
+        <v>1</v>
+      </c>
+      <c r="P11" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="R11" s="11"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="10"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="51">
+        <v>7</v>
+      </c>
+      <c r="D12" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="48">
+        <v>13</v>
+      </c>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48">
+        <v>0.75</v>
+      </c>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48">
+        <v>2.25</v>
+      </c>
+      <c r="M12" s="48">
+        <v>8</v>
+      </c>
+      <c r="N12" s="48">
+        <v>2</v>
+      </c>
+      <c r="O12" s="18"/>
+      <c r="P12" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="W12" s="10"/>
+    </row>
+    <row r="13" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="24"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="51">
+        <v>8</v>
+      </c>
+      <c r="D13" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>To Do</v>
+      </c>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="W13" s="10"/>
+    </row>
+    <row r="14" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" s="24"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="51">
+        <v>9</v>
+      </c>
+      <c r="D14" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="48">
+        <v>4</v>
+      </c>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="18">
+        <v>4</v>
+      </c>
+      <c r="P14" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="97" t="s">
+        <v>44</v>
+      </c>
+      <c r="S14" s="100"/>
+      <c r="T14" s="100"/>
+      <c r="U14" s="100"/>
+      <c r="V14" s="101"/>
+      <c r="W14" s="10"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="51">
+        <v>10</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="48">
+        <v>1</v>
+      </c>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48">
+        <v>1</v>
+      </c>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="Q15" s="44"/>
+      <c r="R15" s="70"/>
+      <c r="S15" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="T15" s="85"/>
+      <c r="U15" s="44">
+        <f>SUM(E6:E25)</f>
+        <v>45</v>
+      </c>
+      <c r="V15" s="71"/>
+      <c r="W15" s="10"/>
+    </row>
+    <row r="16" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="24"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="51">
+        <v>11</v>
+      </c>
+      <c r="D16" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="48">
+        <v>2</v>
+      </c>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48">
+        <v>2</v>
+      </c>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="Q16" s="44"/>
+      <c r="R16" s="70"/>
+      <c r="S16" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="T16" s="86"/>
+      <c r="U16" s="44">
+        <f>SUMIF(F6:O25,"&lt;0")*-1</f>
+        <v>4</v>
+      </c>
+      <c r="V16" s="71"/>
+      <c r="W16" s="10"/>
+    </row>
+    <row r="17" spans="1:24" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="24"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="51">
+        <v>12</v>
+      </c>
+      <c r="D17" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="48">
+        <v>1</v>
+      </c>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48">
+        <v>1</v>
+      </c>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="82" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="Q17" s="44"/>
+      <c r="R17" s="87" t="s">
+        <v>35</v>
+      </c>
+      <c r="S17" s="88"/>
+      <c r="T17" s="88"/>
+      <c r="U17" s="75">
+        <f>SUM(U15,U16)</f>
+        <v>49</v>
+      </c>
+      <c r="V17" s="71"/>
+      <c r="W17" s="10"/>
+    </row>
+    <row r="18" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="24"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="51">
+        <v>13</v>
+      </c>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="83"/>
+      <c r="P18" s="84" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q18" s="44"/>
+      <c r="R18" s="72"/>
+      <c r="S18" s="41"/>
+      <c r="T18" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="U18" s="73"/>
+      <c r="V18" s="74"/>
+      <c r="W18" s="10"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A19" s="24"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="51">
+        <v>14</v>
+      </c>
+      <c r="D19" s="65"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="48"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q19" s="44"/>
+      <c r="W19" s="10"/>
+    </row>
+    <row r="20" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="24"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="51">
+        <v>15</v>
+      </c>
+      <c r="D20" s="69"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q20" s="44"/>
+      <c r="W20" s="10"/>
+    </row>
+    <row r="21" spans="1:24" ht="18" x14ac:dyDescent="0.35">
+      <c r="A21" s="24"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="51">
+        <v>16</v>
+      </c>
+      <c r="D21" s="69"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q21" s="44"/>
+      <c r="R21" s="97" t="s">
+        <v>43</v>
+      </c>
+      <c r="S21" s="98"/>
+      <c r="T21" s="98"/>
+      <c r="U21" s="98"/>
+      <c r="V21" s="99"/>
+      <c r="W21" s="10"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A22" s="24"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="51">
+        <v>17</v>
+      </c>
+      <c r="D22" s="65"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q22" s="44"/>
+      <c r="R22" s="70"/>
+      <c r="S22" s="85" t="s">
+        <v>39</v>
+      </c>
+      <c r="T22" s="85"/>
+      <c r="U22" s="44">
+        <f>SUMIF(F6:J25,"&gt;0")</f>
+        <v>13.25</v>
+      </c>
+      <c r="V22" s="71"/>
+      <c r="W22" s="10"/>
+    </row>
+    <row r="23" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="24"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="51">
+        <v>18</v>
+      </c>
+      <c r="D23" s="65"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q23" s="44"/>
+      <c r="R23" s="70"/>
+      <c r="S23" s="86" t="s">
+        <v>38</v>
+      </c>
+      <c r="T23" s="86"/>
+      <c r="U23" s="78">
+        <f>SUMIF(K6:O25,"&gt;0")</f>
+        <v>35.75</v>
+      </c>
+      <c r="V23" s="71"/>
+      <c r="W23" s="10"/>
+    </row>
+    <row r="24" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="24"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="51">
+        <v>19</v>
+      </c>
+      <c r="D24" s="65"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q24" s="44"/>
+      <c r="R24" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="S24" s="88"/>
+      <c r="T24" s="88"/>
+      <c r="U24" s="77">
+        <f>SUM(U22,U23)</f>
+        <v>49</v>
+      </c>
+      <c r="V24" s="71"/>
+      <c r="W24" s="10"/>
+    </row>
+    <row r="25" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="24"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="51">
+        <v>20</v>
+      </c>
+      <c r="D25" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="19">
+        <v>7</v>
+      </c>
+      <c r="F25" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="H25" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="I25" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="J25" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="K25" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="L25" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="M25" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="N25" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="O25" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="P25" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="Q25" s="44"/>
+      <c r="R25" s="72"/>
+      <c r="S25" s="41"/>
+      <c r="T25" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="U25" s="73"/>
+      <c r="V25" s="74"/>
+      <c r="W25" s="10"/>
+    </row>
+    <row r="26" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="24"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="79" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="68">
+        <f>SUM(E6:E25)</f>
+        <v>45</v>
+      </c>
+      <c r="F26" s="50">
+        <f>E26-SUM(F6:F25)</f>
+        <v>44.5</v>
+      </c>
+      <c r="G26" s="50">
+        <f>F26-SUM(G6:G25)</f>
+        <v>47</v>
+      </c>
+      <c r="H26" s="50">
+        <f t="shared" ref="H26:O26" si="1">G26-SUM(H6:H25)</f>
+        <v>41.5</v>
+      </c>
+      <c r="I26" s="50">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J26" s="50">
+        <f t="shared" si="1"/>
+        <v>35.75</v>
+      </c>
+      <c r="K26" s="50">
+        <f t="shared" si="1"/>
+        <v>29.25</v>
+      </c>
+      <c r="L26" s="50">
+        <f t="shared" si="1"/>
+        <v>25.5</v>
+      </c>
+      <c r="M26" s="50">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="N26" s="50">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+      <c r="O26" s="50">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P26" s="53"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="44"/>
+      <c r="T26" s="44"/>
+      <c r="U26" s="44"/>
+      <c r="V26" s="44"/>
+      <c r="W26" s="10"/>
+    </row>
+    <row r="27" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="24"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="38">
+        <f>E26</f>
+        <v>45</v>
+      </c>
+      <c r="F27" s="39">
+        <f t="shared" ref="F27:O27" si="2">E27-($E$26/10)</f>
+        <v>40.5</v>
+      </c>
+      <c r="G27" s="39">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="H27" s="39">
+        <f t="shared" si="2"/>
+        <v>31.5</v>
+      </c>
+      <c r="I27" s="39">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="J27" s="39">
+        <f t="shared" si="2"/>
+        <v>22.5</v>
+      </c>
+      <c r="K27" s="39">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="L27" s="39">
+        <f t="shared" si="2"/>
+        <v>13.5</v>
+      </c>
+      <c r="M27" s="39">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="N27" s="39">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+      <c r="O27" s="40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P27" s="44"/>
+      <c r="Q27" s="44"/>
+      <c r="R27" s="44"/>
+      <c r="S27" s="44"/>
+      <c r="T27" s="44"/>
+      <c r="U27" s="44"/>
+      <c r="V27" s="44"/>
+      <c r="W27" s="10"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A28" s="24"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="44"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="44"/>
+      <c r="P28" s="44"/>
+      <c r="Q28" s="44"/>
+      <c r="R28" s="44"/>
+      <c r="S28" s="44"/>
+      <c r="T28" s="44"/>
+      <c r="U28" s="44"/>
+      <c r="V28" s="44"/>
+      <c r="W28" s="10"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A29" s="24"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="44"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="44"/>
+      <c r="Q29" s="44"/>
+      <c r="R29" s="44"/>
+      <c r="S29" s="44"/>
+      <c r="T29" s="44"/>
+      <c r="U29" s="44"/>
+      <c r="V29" s="44"/>
+      <c r="W29" s="10"/>
+    </row>
+    <row r="30" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="24"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="41"/>
+      <c r="W30" s="13"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A31" s="24"/>
+      <c r="X31" s="15"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A32" s="24"/>
+      <c r="X32" s="15"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A33" s="24"/>
+      <c r="X33" s="15"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A34" s="24"/>
+      <c r="X34" s="15"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A35" s="24"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
+      <c r="M35" s="44"/>
+      <c r="N35" s="44"/>
+      <c r="O35" s="44"/>
+      <c r="P35" s="44"/>
+      <c r="Q35" s="44"/>
+      <c r="R35" s="44"/>
+      <c r="S35" s="44"/>
+      <c r="T35" s="44"/>
+      <c r="U35" s="44"/>
+      <c r="V35" s="44"/>
+      <c r="W35" s="8"/>
+      <c r="X35" s="15"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A36" s="24"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
+      <c r="L36" s="44"/>
+      <c r="M36" s="44"/>
+      <c r="N36" s="44"/>
+      <c r="O36" s="44"/>
+      <c r="P36" s="44"/>
+      <c r="Q36" s="44"/>
+      <c r="R36" s="44"/>
+      <c r="S36" s="44"/>
+      <c r="T36" s="44"/>
+      <c r="U36" s="44"/>
+      <c r="V36" s="44"/>
+      <c r="W36" s="8"/>
+      <c r="X36" s="15"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A37" s="24"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="44"/>
+      <c r="N37" s="44"/>
+      <c r="O37" s="44"/>
+      <c r="P37" s="44"/>
+      <c r="Q37" s="44"/>
+      <c r="R37" s="44"/>
+      <c r="S37" s="44"/>
+      <c r="T37" s="44"/>
+      <c r="U37" s="44"/>
+      <c r="V37" s="44"/>
+      <c r="W37" s="8"/>
+      <c r="X37" s="15"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A38" s="24"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="44"/>
+      <c r="L38" s="44"/>
+      <c r="M38" s="44"/>
+      <c r="N38" s="44"/>
+      <c r="O38" s="44"/>
+      <c r="P38" s="44"/>
+      <c r="Q38" s="44"/>
+      <c r="R38" s="44"/>
+      <c r="S38" s="44"/>
+      <c r="T38" s="44"/>
+      <c r="U38" s="44"/>
+      <c r="V38" s="44"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="15"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A39" s="24"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44"/>
+      <c r="L39" s="44"/>
+      <c r="M39" s="44"/>
+      <c r="N39" s="44"/>
+      <c r="O39" s="44"/>
+      <c r="P39" s="44"/>
+      <c r="Q39" s="44"/>
+      <c r="R39" s="44"/>
+      <c r="S39" s="44"/>
+      <c r="T39" s="44"/>
+      <c r="U39" s="44"/>
+      <c r="V39" s="44"/>
+      <c r="W39" s="8"/>
+      <c r="X39" s="15"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A40" s="24"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
+      <c r="U40" s="8"/>
+      <c r="W40" s="8"/>
+      <c r="X40" s="15"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A41" s="24"/>
+      <c r="B41" s="15"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A42" s="24"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="24"/>
+      <c r="N42" s="24"/>
+      <c r="O42" s="24"/>
+      <c r="P42" s="24"/>
+      <c r="Q42" s="24"/>
+      <c r="R42" s="24"/>
+      <c r="S42" s="24"/>
+      <c r="T42" s="24"/>
+      <c r="U42" s="24"/>
+      <c r="V42" s="24"/>
+      <c r="W42" s="24"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="C4:O27"/>
+  <mergeCells count="13">
+    <mergeCell ref="R14:V14"/>
+    <mergeCell ref="B1:W1"/>
+    <mergeCell ref="B2:W2"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="R6:V6"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="R21:V21"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S23:T23"/>
+  </mergeCells>
+  <conditionalFormatting sqref="P6:P25">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Incomplete">
+      <formula>NOT(ISERROR(SEARCH("Incomplete",P6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",P6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P6:P25">
+    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E26">
+      <formula1>-24</formula1>
+      <formula2>50</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E25">
+      <formula1>0</formula1>
+      <formula2>25</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E17 F12:N17 E19:N24">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H26:O27 E27 F25:G27 H25:N25 K6:N11 F8:J11 O6:O17 O19:O25">
+      <formula1>-24</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S9:S10">
+      <formula1>-100</formula1>
+      <formula2>1000000</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S8">
+      <formula1>0</formula1>
+      <formula2>1000000</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="45" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;C
+</oddHeader>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" stopIfTrue="1" operator="containsText" id="{710BAB5E-01CD-4EFB-BA44-82D5DFDE9064}">
+            <xm:f>NOT(ISERROR(SEARCH("To Do",P6)))</xm:f>
+            <xm:f>"To Do"</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="1"/>
+              </font>
+              <fill>
+                <patternFill patternType="none">
+                  <bgColor auto="1"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>P6:P25</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:X42"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="66.5546875" customWidth="1"/>
+    <col min="5" max="15" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" customWidth="1"/>
+    <col min="21" max="21" width="6" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" customWidth="1"/>
+    <col min="24" max="24" width="25.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="49.8" x14ac:dyDescent="0.8">
+      <c r="A1" s="24"/>
+      <c r="B1" s="89" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="89"/>
+      <c r="T1" s="89"/>
+      <c r="U1" s="89"/>
+      <c r="V1" s="89"/>
+      <c r="W1" s="89"/>
+    </row>
+    <row r="2" spans="1:23" ht="33" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="24"/>
+      <c r="B2" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="90"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="90"/>
+      <c r="W2" s="90"/>
+    </row>
+    <row r="3" spans="1:23" s="1" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="22"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="91" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="96"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="32"/>
+    </row>
+    <row r="4" spans="1:23" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="34"/>
+      <c r="F4" s="43">
+        <v>42844</v>
+      </c>
+      <c r="G4" s="43">
+        <v>42845</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="42">
+        <v>42849</v>
+      </c>
+      <c r="J4" s="42">
+        <v>42850</v>
+      </c>
+      <c r="K4" s="42">
+        <v>42851</v>
+      </c>
+      <c r="L4" s="42">
+        <v>42852</v>
+      </c>
+      <c r="M4" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="N4" s="43">
+        <v>42856</v>
+      </c>
+      <c r="O4" s="58">
+        <v>42857</v>
+      </c>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="W4" s="27"/>
+    </row>
+    <row r="5" spans="1:23" s="2" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="23"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="W5" s="27"/>
+    </row>
+    <row r="6" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="24"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="17">
+        <v>1</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="63">
+        <v>3</v>
+      </c>
+      <c r="F6" s="63">
+        <v>3</v>
+      </c>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="76" t="str">
+        <f t="shared" ref="P6:P25" si="0">IF(D6="","-",(IF(COUNT(E6:O6) = 0,"To Do",IF(E6&gt;SUM(F6:O6),"Incomplete","Done"))))</f>
+        <v>Done</v>
+      </c>
+      <c r="R6" s="97" t="s">
+        <v>4</v>
+      </c>
+      <c r="S6" s="100"/>
+      <c r="T6" s="100"/>
+      <c r="U6" s="100"/>
+      <c r="V6" s="101"/>
+      <c r="W6" s="10"/>
+    </row>
+    <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="24"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="17">
+        <v>2</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>To Do</v>
+      </c>
+      <c r="R7" s="9"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+    </row>
+    <row r="8" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="17">
+        <v>3</v>
+      </c>
+      <c r="D8" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>Incomplete</v>
+      </c>
+      <c r="R8" s="9"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A9" s="24"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="17">
+        <v>4</v>
+      </c>
+      <c r="D9" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>To Do</v>
+      </c>
+      <c r="R9" s="9"/>
+      <c r="S9" s="45"/>
+      <c r="T9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A10" s="24"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="17">
+        <v>5</v>
+      </c>
+      <c r="D10" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>To Do</v>
+      </c>
+      <c r="R10" s="9"/>
+      <c r="S10" s="46"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+    </row>
+    <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="24"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="47">
+        <v>6</v>
+      </c>
+      <c r="D11" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>To Do</v>
+      </c>
+      <c r="R11" s="11"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="10"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="51">
+        <v>7</v>
+      </c>
+      <c r="D12" s="65"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="W12" s="10"/>
+    </row>
+    <row r="13" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="24"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="51">
+        <v>8</v>
+      </c>
+      <c r="D13" s="65"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="W13" s="10"/>
+    </row>
+    <row r="14" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" s="24"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="51">
+        <v>9</v>
+      </c>
+      <c r="D14" s="65"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="97" t="s">
+        <v>44</v>
+      </c>
+      <c r="S14" s="100"/>
+      <c r="T14" s="100"/>
+      <c r="U14" s="100"/>
+      <c r="V14" s="101"/>
+      <c r="W14" s="10"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="51">
+        <v>10</v>
+      </c>
+      <c r="D15" s="65"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q15" s="44"/>
+      <c r="R15" s="70"/>
+      <c r="S15" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="T15" s="85"/>
+      <c r="U15" s="44">
+        <f>SUM(E6:E25)</f>
+        <v>12</v>
+      </c>
+      <c r="V15" s="71"/>
+      <c r="W15" s="10"/>
+    </row>
+    <row r="16" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="24"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="51">
+        <v>11</v>
+      </c>
+      <c r="D16" s="65"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q16" s="44"/>
+      <c r="R16" s="70"/>
+      <c r="S16" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="T16" s="86"/>
+      <c r="U16" s="44">
+        <f>SUMIF(F6:O25,"&lt;0")*-1</f>
+        <v>0</v>
+      </c>
+      <c r="V16" s="71"/>
+      <c r="W16" s="10"/>
+    </row>
+    <row r="17" spans="1:24" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="24"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="51">
+        <v>12</v>
+      </c>
+      <c r="D17" s="65"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q17" s="44"/>
+      <c r="R17" s="87" t="s">
+        <v>35</v>
+      </c>
+      <c r="S17" s="88"/>
+      <c r="T17" s="88"/>
+      <c r="U17" s="75">
+        <f>SUM(U15,U16)</f>
+        <v>12</v>
+      </c>
+      <c r="V17" s="71"/>
+      <c r="W17" s="10"/>
+    </row>
+    <row r="18" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="24"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="51">
+        <v>13</v>
+      </c>
+      <c r="D18" s="65"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q18" s="44"/>
+      <c r="R18" s="72"/>
+      <c r="S18" s="41"/>
+      <c r="T18" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="U18" s="73"/>
+      <c r="V18" s="74"/>
+      <c r="W18" s="10"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A19" s="24"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="51">
+        <v>14</v>
+      </c>
+      <c r="D19" s="65"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="48"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q19" s="44"/>
+      <c r="W19" s="10"/>
+    </row>
+    <row r="20" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="24"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="51">
+        <v>15</v>
+      </c>
+      <c r="D20" s="69"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q20" s="44"/>
+      <c r="W20" s="10"/>
+    </row>
+    <row r="21" spans="1:24" ht="18" x14ac:dyDescent="0.35">
+      <c r="A21" s="24"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="51">
+        <v>16</v>
+      </c>
+      <c r="D21" s="69"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q21" s="44"/>
+      <c r="R21" s="97" t="s">
+        <v>43</v>
+      </c>
+      <c r="S21" s="98"/>
+      <c r="T21" s="98"/>
+      <c r="U21" s="98"/>
+      <c r="V21" s="99"/>
+      <c r="W21" s="10"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A22" s="24"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="51">
+        <v>17</v>
+      </c>
+      <c r="D22" s="65"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q22" s="44"/>
+      <c r="R22" s="70"/>
+      <c r="S22" s="85" t="s">
+        <v>39</v>
+      </c>
+      <c r="T22" s="85"/>
+      <c r="U22" s="44">
+        <f>SUMIF(F6:J25,"&gt;0")</f>
+        <v>3.5</v>
+      </c>
+      <c r="V22" s="71"/>
+      <c r="W22" s="10"/>
+    </row>
+    <row r="23" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="24"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="51">
+        <v>18</v>
+      </c>
+      <c r="D23" s="65"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q23" s="44"/>
+      <c r="R23" s="70"/>
+      <c r="S23" s="86" t="s">
+        <v>38</v>
+      </c>
+      <c r="T23" s="86"/>
+      <c r="U23" s="78">
+        <f>SUMIF(K6:O25,"&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="V23" s="71"/>
+      <c r="W23" s="10"/>
+    </row>
+    <row r="24" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="24"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="51">
+        <v>19</v>
+      </c>
+      <c r="D24" s="65"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="Q24" s="44"/>
+      <c r="R24" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="S24" s="88"/>
+      <c r="T24" s="88"/>
+      <c r="U24" s="77">
+        <f>SUM(U22,U23)</f>
+        <v>3.5</v>
+      </c>
+      <c r="V24" s="71"/>
+      <c r="W24" s="10"/>
+    </row>
+    <row r="25" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="24"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="51">
+        <v>20</v>
+      </c>
+      <c r="D25" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="19">
+        <v>7</v>
+      </c>
+      <c r="F25" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="76" t="str">
+        <f t="shared" si="0"/>
+        <v>Incomplete</v>
+      </c>
+      <c r="Q25" s="44"/>
+      <c r="R25" s="72"/>
+      <c r="S25" s="41"/>
+      <c r="T25" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="U25" s="73"/>
+      <c r="V25" s="74"/>
+      <c r="W25" s="10"/>
+    </row>
+    <row r="26" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="24"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="80" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="68">
+        <f>SUM(E6:E25)</f>
+        <v>12</v>
+      </c>
+      <c r="F26" s="50">
+        <f>E26-SUM(F6:F25)</f>
+        <v>8.5</v>
+      </c>
+      <c r="G26" s="50">
+        <f>F26-SUM(G6:G25)</f>
+        <v>8.5</v>
+      </c>
+      <c r="H26" s="50">
+        <f t="shared" ref="H26:O26" si="1">G26-SUM(H6:H25)</f>
+        <v>8.5</v>
+      </c>
+      <c r="I26" s="50">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="J26" s="50">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="K26" s="50">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="L26" s="50">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="M26" s="50">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="N26" s="50">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="O26" s="50">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="P26" s="53"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="44"/>
+      <c r="T26" s="44"/>
+      <c r="U26" s="44"/>
+      <c r="V26" s="44"/>
+      <c r="W26" s="10"/>
+    </row>
+    <row r="27" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="24"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="38">
+        <f>E26</f>
+        <v>12</v>
+      </c>
+      <c r="F27" s="39">
+        <f t="shared" ref="F27:O27" si="2">E27-($E$26/10)</f>
+        <v>10.8</v>
+      </c>
+      <c r="G27" s="39">
+        <f t="shared" si="2"/>
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="H27" s="39">
+        <f t="shared" si="2"/>
+        <v>8.4000000000000021</v>
+      </c>
+      <c r="I27" s="39">
+        <f t="shared" si="2"/>
+        <v>7.200000000000002</v>
+      </c>
+      <c r="J27" s="39">
+        <f t="shared" si="2"/>
+        <v>6.0000000000000018</v>
+      </c>
+      <c r="K27" s="39">
+        <f t="shared" si="2"/>
+        <v>4.8000000000000016</v>
+      </c>
+      <c r="L27" s="39">
+        <f t="shared" si="2"/>
+        <v>3.6000000000000014</v>
+      </c>
+      <c r="M27" s="39">
+        <f t="shared" si="2"/>
+        <v>2.4000000000000012</v>
+      </c>
+      <c r="N27" s="39">
+        <f t="shared" si="2"/>
+        <v>1.2000000000000013</v>
+      </c>
+      <c r="O27" s="40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P27" s="44"/>
+      <c r="Q27" s="44"/>
+      <c r="R27" s="44"/>
+      <c r="S27" s="44"/>
+      <c r="T27" s="44"/>
+      <c r="U27" s="44"/>
+      <c r="V27" s="44"/>
+      <c r="W27" s="10"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A28" s="24"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="44"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="44"/>
+      <c r="P28" s="44"/>
+      <c r="Q28" s="44"/>
+      <c r="R28" s="44"/>
+      <c r="S28" s="44"/>
+      <c r="T28" s="44"/>
+      <c r="U28" s="44"/>
+      <c r="V28" s="44"/>
+      <c r="W28" s="10"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A29" s="24"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="44"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="44"/>
+      <c r="Q29" s="44"/>
+      <c r="R29" s="44"/>
+      <c r="S29" s="44"/>
+      <c r="T29" s="44"/>
+      <c r="U29" s="44"/>
+      <c r="V29" s="44"/>
+      <c r="W29" s="10"/>
+    </row>
+    <row r="30" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="24"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="41"/>
+      <c r="W30" s="13"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A31" s="24"/>
+      <c r="X31" s="15"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A32" s="24"/>
+      <c r="X32" s="15"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A33" s="24"/>
+      <c r="X33" s="15"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A34" s="24"/>
+      <c r="X34" s="15"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A35" s="24"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
+      <c r="M35" s="44"/>
+      <c r="N35" s="44"/>
+      <c r="O35" s="44"/>
+      <c r="P35" s="44"/>
+      <c r="Q35" s="44"/>
+      <c r="R35" s="44"/>
+      <c r="S35" s="44"/>
+      <c r="T35" s="44"/>
+      <c r="U35" s="44"/>
+      <c r="V35" s="44"/>
+      <c r="W35" s="8"/>
+      <c r="X35" s="15"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A36" s="24"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
+      <c r="L36" s="44"/>
+      <c r="M36" s="44"/>
+      <c r="N36" s="44"/>
+      <c r="O36" s="44"/>
+      <c r="P36" s="44"/>
+      <c r="Q36" s="44"/>
+      <c r="R36" s="44"/>
+      <c r="S36" s="44"/>
+      <c r="T36" s="44"/>
+      <c r="U36" s="44"/>
+      <c r="V36" s="44"/>
+      <c r="W36" s="8"/>
+      <c r="X36" s="15"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A37" s="24"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="44"/>
+      <c r="N37" s="44"/>
+      <c r="O37" s="44"/>
+      <c r="P37" s="44"/>
+      <c r="Q37" s="44"/>
+      <c r="R37" s="44"/>
+      <c r="S37" s="44"/>
+      <c r="T37" s="44"/>
+      <c r="U37" s="44"/>
+      <c r="V37" s="44"/>
+      <c r="W37" s="8"/>
+      <c r="X37" s="15"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A38" s="24"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="44"/>
+      <c r="L38" s="44"/>
+      <c r="M38" s="44"/>
+      <c r="N38" s="44"/>
+      <c r="O38" s="44"/>
+      <c r="P38" s="44"/>
+      <c r="Q38" s="44"/>
+      <c r="R38" s="44"/>
+      <c r="S38" s="44"/>
+      <c r="T38" s="44"/>
+      <c r="U38" s="44"/>
+      <c r="V38" s="44"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="15"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A39" s="24"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44"/>
+      <c r="L39" s="44"/>
+      <c r="M39" s="44"/>
+      <c r="N39" s="44"/>
+      <c r="O39" s="44"/>
+      <c r="P39" s="44"/>
+      <c r="Q39" s="44"/>
+      <c r="R39" s="44"/>
+      <c r="S39" s="44"/>
+      <c r="T39" s="44"/>
+      <c r="U39" s="44"/>
+      <c r="V39" s="44"/>
+      <c r="W39" s="8"/>
+      <c r="X39" s="15"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A40" s="24"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
+      <c r="U40" s="8"/>
+      <c r="W40" s="8"/>
+      <c r="X40" s="15"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A41" s="24"/>
+      <c r="B41" s="15"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A42" s="24"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="24"/>
+      <c r="N42" s="24"/>
+      <c r="O42" s="24"/>
+      <c r="P42" s="24"/>
+      <c r="Q42" s="24"/>
+      <c r="R42" s="24"/>
+      <c r="S42" s="24"/>
+      <c r="T42" s="24"/>
+      <c r="U42" s="24"/>
+      <c r="V42" s="24"/>
+      <c r="W42" s="24"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="C4:O27"/>
+  <mergeCells count="13">
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="R21:V21"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="R14:V14"/>
+    <mergeCell ref="B1:W1"/>
+    <mergeCell ref="B2:W2"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="R6:V6"/>
+  </mergeCells>
+  <conditionalFormatting sqref="P6:P25">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Incomplete">
+      <formula>NOT(ISERROR(SEARCH("Incomplete",P6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",P6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P6:P25">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S8">
+      <formula1>0</formula1>
+      <formula2>1000000</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S9:S10">
+      <formula1>-100</formula1>
+      <formula2>1000000</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H26:O27 E27 F8:J12 O6:O25 F25:G27 H25:N25 K6:N12">
+      <formula1>-24</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E24 F13:N24">
+      <formula1>0</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E25">
+      <formula1>0</formula1>
+      <formula2>25</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E26">
+      <formula1>-24</formula1>
+      <formula2>50</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="45" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;C
+</oddHeader>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" stopIfTrue="1" operator="containsText" id="{0E58A550-5457-469D-AFC6-5415EA4A3034}">
+            <xm:f>NOT(ISERROR(SEARCH("To Do",P6)))</xm:f>
+            <xm:f>"To Do"</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="1"/>
+              </font>
+              <fill>
+                <patternFill patternType="none">
+                  <bgColor auto="1"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>P6:P25</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated burndown chart with Heymond's logs
</commit_message>
<xml_diff>
--- a/burndown/Team Blue Burndown Chart.xlsx
+++ b/burndown/Team Blue Burndown Chart.xlsx
@@ -429,7 +429,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="68">
   <si>
     <t>Initial 
 Estimate</t>
@@ -631,6 +631,9 @@
   </si>
   <si>
     <t>Networking (still needs estimate)</t>
+  </si>
+  <si>
+    <t>Last minute adjustments to Android app for demo</t>
   </si>
 </sst>
 </file>
@@ -2086,34 +2089,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>47.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>44.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>41.5</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.75</c:v>
+                  <c:v>38.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.25</c:v>
+                  <c:v>32.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25.5</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -2161,34 +2164,34 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.5</c:v>
+                  <c:v>43.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36</c:v>
+                  <c:v>38.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.5</c:v>
+                  <c:v>33.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>28.800000000000008</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.5</c:v>
+                  <c:v>24.000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18</c:v>
+                  <c:v>19.200000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.5</c:v>
+                  <c:v>14.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>9.600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.5</c:v>
+                  <c:v>4.8000000000000052</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -2396,7 +2399,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8.5</c:v>
@@ -2471,34 +2474,34 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.8</c:v>
+                  <c:v>21.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.6000000000000014</c:v>
+                  <c:v>19.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.4000000000000021</c:v>
+                  <c:v>16.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.200000000000002</c:v>
+                  <c:v>14.400000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0000000000000018</c:v>
+                  <c:v>12.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.8000000000000016</c:v>
+                  <c:v>9.6000000000000032</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.6000000000000014</c:v>
+                  <c:v>7.2000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.4000000000000012</c:v>
+                  <c:v>4.8000000000000025</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2000000000000013</c:v>
+                  <c:v>2.4000000000000026</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -4572,7 +4575,7 @@
   <dimension ref="A1:X42"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5001,7 +5004,7 @@
         <v>57</v>
       </c>
       <c r="E12" s="48">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F12" s="48"/>
       <c r="G12" s="48"/>
@@ -5020,7 +5023,9 @@
       <c r="N12" s="48">
         <v>2</v>
       </c>
-      <c r="O12" s="18"/>
+      <c r="O12" s="18">
+        <v>3</v>
+      </c>
       <c r="P12" s="76" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
@@ -5132,7 +5137,7 @@
       <c r="T15" s="85"/>
       <c r="U15" s="44">
         <f>SUM(E6:E25)</f>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="V15" s="71"/>
       <c r="W15" s="10"/>
@@ -5214,7 +5219,7 @@
       <c r="T17" s="88"/>
       <c r="U17" s="75">
         <f>SUM(U15,U16)</f>
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="V17" s="71"/>
       <c r="W17" s="10"/>
@@ -5398,7 +5403,7 @@
       <c r="T23" s="86"/>
       <c r="U23" s="78">
         <f>SUMIF(K6:O25,"&gt;0")</f>
-        <v>35.75</v>
+        <v>38.75</v>
       </c>
       <c r="V23" s="71"/>
       <c r="W23" s="10"/>
@@ -5433,7 +5438,7 @@
       <c r="T24" s="88"/>
       <c r="U24" s="77">
         <f>SUM(U22,U23)</f>
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="V24" s="71"/>
       <c r="W24" s="10"/>
@@ -5503,43 +5508,43 @@
       </c>
       <c r="E26" s="68">
         <f>SUM(E6:E25)</f>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F26" s="50">
         <f>E26-SUM(F6:F25)</f>
-        <v>44.5</v>
+        <v>47.5</v>
       </c>
       <c r="G26" s="50">
         <f>F26-SUM(G6:G25)</f>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H26" s="50">
         <f t="shared" ref="H26:O26" si="1">G26-SUM(H6:H25)</f>
-        <v>41.5</v>
+        <v>44.5</v>
       </c>
       <c r="I26" s="50">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J26" s="50">
         <f t="shared" si="1"/>
-        <v>35.75</v>
+        <v>38.75</v>
       </c>
       <c r="K26" s="50">
         <f t="shared" si="1"/>
-        <v>29.25</v>
+        <v>32.25</v>
       </c>
       <c r="L26" s="50">
         <f t="shared" si="1"/>
-        <v>25.5</v>
+        <v>28.5</v>
       </c>
       <c r="M26" s="50">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N26" s="50">
         <f t="shared" si="1"/>
-        <v>6.5</v>
+        <v>9.5</v>
       </c>
       <c r="O26" s="50">
         <f t="shared" si="1"/>
@@ -5563,43 +5568,43 @@
       </c>
       <c r="E27" s="38">
         <f>E26</f>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F27" s="39">
         <f t="shared" ref="F27:O27" si="2">E27-($E$26/10)</f>
-        <v>40.5</v>
+        <v>43.2</v>
       </c>
       <c r="G27" s="39">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>38.400000000000006</v>
       </c>
       <c r="H27" s="39">
         <f t="shared" si="2"/>
-        <v>31.5</v>
+        <v>33.600000000000009</v>
       </c>
       <c r="I27" s="39">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>28.800000000000008</v>
       </c>
       <c r="J27" s="39">
         <f t="shared" si="2"/>
-        <v>22.5</v>
+        <v>24.000000000000007</v>
       </c>
       <c r="K27" s="39">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>19.200000000000006</v>
       </c>
       <c r="L27" s="39">
         <f t="shared" si="2"/>
-        <v>13.5</v>
+        <v>14.400000000000006</v>
       </c>
       <c r="M27" s="39">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>9.600000000000005</v>
       </c>
       <c r="N27" s="39">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>4.8000000000000052</v>
       </c>
       <c r="O27" s="40">
         <f t="shared" si="2"/>
@@ -5987,8 +5992,8 @@
   </sheetPr>
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6224,11 +6229,15 @@
       <c r="C7" s="17">
         <v>2</v>
       </c>
-      <c r="D7" s="65" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
+      <c r="D7" s="69" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="63">
+        <v>12</v>
+      </c>
+      <c r="F7" s="63">
+        <v>12</v>
+      </c>
       <c r="G7" s="63"/>
       <c r="H7" s="63"/>
       <c r="I7" s="63"/>
@@ -6240,7 +6249,7 @@
       <c r="O7" s="18"/>
       <c r="P7" s="76" t="str">
         <f t="shared" si="0"/>
-        <v>To Do</v>
+        <v>Done</v>
       </c>
       <c r="R7" s="9"/>
       <c r="S7" s="14"/>
@@ -6255,8 +6264,8 @@
       <c r="C8" s="17">
         <v>3</v>
       </c>
-      <c r="D8" s="69" t="s">
-        <v>62</v>
+      <c r="D8" s="65" t="s">
+        <v>63</v>
       </c>
       <c r="E8" s="3">
         <v>2</v>
@@ -6289,8 +6298,8 @@
       <c r="C9" s="17">
         <v>4</v>
       </c>
-      <c r="D9" s="65" t="s">
-        <v>66</v>
+      <c r="D9" s="69" t="s">
+        <v>62</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -6322,7 +6331,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="65" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -6353,10 +6362,10 @@
         <v>6</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
+        <v>65</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="48"/>
       <c r="H11" s="48"/>
       <c r="I11" s="48"/>
@@ -6383,7 +6392,9 @@
       <c r="C12" s="51">
         <v>7</v>
       </c>
-      <c r="D12" s="65"/>
+      <c r="D12" s="65" t="s">
+        <v>64</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -6397,7 +6408,7 @@
       <c r="O12" s="18"/>
       <c r="P12" s="76" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>To Do</v>
       </c>
       <c r="W12" s="10"/>
     </row>
@@ -6407,9 +6418,9 @@
       <c r="C13" s="51">
         <v>8</v>
       </c>
-      <c r="D13" s="65"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="48"/>
       <c r="H13" s="48"/>
       <c r="I13" s="48"/>
@@ -6437,8 +6448,8 @@
         <v>9</v>
       </c>
       <c r="D14" s="65"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
       <c r="G14" s="48"/>
       <c r="H14" s="48"/>
       <c r="I14" s="48"/>
@@ -6469,8 +6480,8 @@
         <v>10</v>
       </c>
       <c r="D15" s="65"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
       <c r="G15" s="48"/>
       <c r="H15" s="48"/>
       <c r="I15" s="48"/>
@@ -6492,7 +6503,7 @@
       <c r="T15" s="85"/>
       <c r="U15" s="44">
         <f>SUM(E6:E25)</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="V15" s="71"/>
       <c r="W15" s="10"/>
@@ -6504,8 +6515,8 @@
         <v>11</v>
       </c>
       <c r="D16" s="65"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="48"/>
       <c r="H16" s="48"/>
       <c r="I16" s="48"/>
@@ -6539,8 +6550,8 @@
         <v>12</v>
       </c>
       <c r="D17" s="65"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="48"/>
       <c r="H17" s="48"/>
       <c r="I17" s="48"/>
@@ -6562,7 +6573,7 @@
       <c r="T17" s="88"/>
       <c r="U17" s="75">
         <f>SUM(U15,U16)</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="V17" s="71"/>
       <c r="W17" s="10"/>
@@ -6711,7 +6722,7 @@
       <c r="T22" s="85"/>
       <c r="U22" s="44">
         <f>SUMIF(F6:J25,"&gt;0")</f>
-        <v>3.5</v>
+        <v>15.5</v>
       </c>
       <c r="V22" s="71"/>
       <c r="W22" s="10"/>
@@ -6781,7 +6792,7 @@
       <c r="T24" s="88"/>
       <c r="U24" s="77">
         <f>SUM(U22,U23)</f>
-        <v>3.5</v>
+        <v>15.5</v>
       </c>
       <c r="V24" s="71"/>
       <c r="W24" s="10"/>
@@ -6833,7 +6844,7 @@
       </c>
       <c r="E26" s="68">
         <f>SUM(E6:E25)</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F26" s="50">
         <f>E26-SUM(F6:F25)</f>
@@ -6893,43 +6904,43 @@
       </c>
       <c r="E27" s="38">
         <f>E26</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F27" s="39">
         <f t="shared" ref="F27:O27" si="2">E27-($E$26/10)</f>
-        <v>10.8</v>
+        <v>21.6</v>
       </c>
       <c r="G27" s="39">
         <f t="shared" si="2"/>
-        <v>9.6000000000000014</v>
+        <v>19.200000000000003</v>
       </c>
       <c r="H27" s="39">
         <f t="shared" si="2"/>
-        <v>8.4000000000000021</v>
+        <v>16.800000000000004</v>
       </c>
       <c r="I27" s="39">
         <f t="shared" si="2"/>
-        <v>7.200000000000002</v>
+        <v>14.400000000000004</v>
       </c>
       <c r="J27" s="39">
         <f t="shared" si="2"/>
-        <v>6.0000000000000018</v>
+        <v>12.000000000000004</v>
       </c>
       <c r="K27" s="39">
         <f t="shared" si="2"/>
-        <v>4.8000000000000016</v>
+        <v>9.6000000000000032</v>
       </c>
       <c r="L27" s="39">
         <f t="shared" si="2"/>
-        <v>3.6000000000000014</v>
+        <v>7.2000000000000028</v>
       </c>
       <c r="M27" s="39">
         <f t="shared" si="2"/>
-        <v>2.4000000000000012</v>
+        <v>4.8000000000000025</v>
       </c>
       <c r="N27" s="39">
         <f t="shared" si="2"/>
-        <v>1.2000000000000013</v>
+        <v>2.4000000000000026</v>
       </c>
       <c r="O27" s="40">
         <f t="shared" si="2"/>
@@ -7262,7 +7273,7 @@
       <formula1>-24</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E24 F13:N24">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13:N24 E8:E12 E14:E24">
       <formula1>0</formula1>
       <formula2>24</formula2>
     </dataValidation>

</xml_diff>